<commit_message>
cambio de motor en escaleta mat 7 tema 11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion11/ESCALETA MA_07_11_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion11/ESCALETA MA_07_11_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11592"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="382">
   <si>
     <t>Asignatura</t>
   </si>
@@ -954,9 +954,6 @@
   </si>
   <si>
     <t>RM_01_02_CO</t>
-  </si>
-  <si>
-    <t>2° ESO</t>
   </si>
   <si>
     <t>Recurso_M5A_01</t>
@@ -1661,22 +1658,13 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1722,6 +1710,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2030,129 +2027,129 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="43.6640625" style="40" customWidth="1"/>
-    <col min="5" max="5" width="67.109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="48.44140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="80.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" style="40" customWidth="1"/>
+    <col min="5" max="5" width="67.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="48.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="80.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="5" customWidth="1"/>
     <col min="9" max="9" width="11" style="49" customWidth="1"/>
-    <col min="10" max="10" width="73.5546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" style="4" customWidth="1"/>
-    <col min="13" max="14" width="9.33203125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="68.5546875" style="5" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" style="5" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" style="71" customWidth="1"/>
+    <col min="10" max="10" width="73.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="4" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="68.5703125" style="5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="5" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="71" customWidth="1"/>
     <col min="18" max="18" width="23" style="72" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" style="72" customWidth="1"/>
-    <col min="20" max="20" width="25.88671875" style="72" customWidth="1"/>
-    <col min="21" max="21" width="21.6640625" style="72" customWidth="1"/>
-    <col min="22" max="22" width="11.44140625" style="4"/>
-    <col min="23" max="24" width="11.44140625" style="5"/>
-    <col min="25" max="16384" width="11.44140625" style="4"/>
+    <col min="19" max="19" width="20.7109375" style="72" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" style="72" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" style="72" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="4"/>
+    <col min="23" max="24" width="11.42578125" style="5"/>
+    <col min="25" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="93" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="83" t="s">
+      <c r="H1" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="I1" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="93" t="s">
+      <c r="J1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="91" t="s">
+      <c r="K1" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="95" t="s">
+      <c r="M1" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="95"/>
-      <c r="O1" s="79" t="s">
+      <c r="N1" s="92"/>
+      <c r="O1" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="P1" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="80" t="s">
+      <c r="Q1" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="82" t="s">
+      <c r="R1" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="80" t="s">
+      <c r="S1" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="81" t="s">
+      <c r="T1" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="80" t="s">
+      <c r="U1" s="97" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="88"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="90"/>
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="85"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="87"/>
       <c r="M2" s="3" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="80"/>
-    </row>
-    <row r="3" spans="1:24" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="97"/>
+    </row>
+    <row r="3" spans="1:24" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -2183,7 +2180,7 @@
         <v>20</v>
       </c>
       <c r="L3" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>55</v>
@@ -2213,7 +2210,7 @@
       <c r="W3" s="16"/>
       <c r="X3" s="16"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2230,7 +2227,7 @@
         <v>133</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>148</v>
@@ -2248,7 +2245,7 @@
         <v>20</v>
       </c>
       <c r="L4" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M4" s="22" t="s">
         <v>58</v>
@@ -2278,7 +2275,7 @@
       <c r="W4" s="16"/>
       <c r="X4" s="16"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -2311,7 +2308,7 @@
         <v>19</v>
       </c>
       <c r="L5" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M5" s="22"/>
       <c r="N5" s="3" t="s">
@@ -2325,21 +2322,21 @@
         <v>7</v>
       </c>
       <c r="R5" s="65" t="s">
+        <v>315</v>
+      </c>
+      <c r="S5" s="64" t="s">
         <v>316</v>
       </c>
-      <c r="S5" s="64" t="s">
+      <c r="T5" s="66" t="s">
         <v>317</v>
       </c>
-      <c r="T5" s="66" t="s">
+      <c r="U5" s="64" t="s">
         <v>318</v>
-      </c>
-      <c r="U5" s="64" t="s">
-        <v>319</v>
       </c>
       <c r="W5" s="16"/>
       <c r="X5" s="16"/>
     </row>
-    <row r="6" spans="1:24" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -2372,7 +2369,7 @@
         <v>19</v>
       </c>
       <c r="L6" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M6" s="14"/>
       <c r="N6" s="73" t="s">
@@ -2386,21 +2383,21 @@
         <v>7</v>
       </c>
       <c r="R6" s="75" t="s">
+        <v>315</v>
+      </c>
+      <c r="S6" s="74" t="s">
         <v>316</v>
       </c>
-      <c r="S6" s="74" t="s">
-        <v>317</v>
-      </c>
       <c r="T6" s="76" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="U6" s="74" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="W6" s="16"/>
       <c r="X6" s="16"/>
     </row>
-    <row r="7" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -2433,7 +2430,7 @@
         <v>19</v>
       </c>
       <c r="L7" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M7" s="22"/>
       <c r="N7" s="6" t="s">
@@ -2447,21 +2444,21 @@
         <v>7</v>
       </c>
       <c r="R7" s="65" t="s">
+        <v>315</v>
+      </c>
+      <c r="S7" s="64" t="s">
         <v>316</v>
       </c>
-      <c r="S7" s="64" t="s">
-        <v>317</v>
-      </c>
       <c r="T7" s="66" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="U7" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="W7" s="16"/>
       <c r="X7" s="16"/>
     </row>
-    <row r="8" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
@@ -2478,7 +2475,7 @@
         <v>134</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>152</v>
@@ -2496,7 +2493,7 @@
         <v>20</v>
       </c>
       <c r="L8" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M8" s="22" t="s">
         <v>55</v>
@@ -2518,7 +2515,7 @@
         <v>298</v>
       </c>
       <c r="T8" s="63" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="U8" s="61" t="s">
         <v>300</v>
@@ -2526,7 +2523,7 @@
       <c r="W8" s="16"/>
       <c r="X8" s="16"/>
     </row>
-    <row r="9" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -2559,7 +2556,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M9" s="22"/>
       <c r="N9" s="6" t="s">
@@ -2581,7 +2578,7 @@
         <v>303</v>
       </c>
       <c r="T9" s="63" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="U9" s="61" t="s">
         <v>307</v>
@@ -2589,7 +2586,7 @@
       <c r="W9" s="16"/>
       <c r="X9" s="16"/>
     </row>
-    <row r="10" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -2606,7 +2603,7 @@
         <v>136</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G10" s="24" t="s">
         <v>154</v>
@@ -2624,7 +2621,7 @@
         <v>20</v>
       </c>
       <c r="L10" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M10" s="22" t="s">
         <v>60</v>
@@ -2654,7 +2651,7 @@
       <c r="W10" s="16"/>
       <c r="X10" s="16"/>
     </row>
-    <row r="11" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -2687,7 +2684,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M11" s="22"/>
       <c r="N11" s="6" t="s">
@@ -2709,7 +2706,7 @@
         <v>306</v>
       </c>
       <c r="T11" s="63" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="U11" s="61" t="s">
         <v>307</v>
@@ -2717,7 +2714,7 @@
       <c r="W11" s="16"/>
       <c r="X11" s="16"/>
     </row>
-    <row r="12" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
@@ -2750,7 +2747,7 @@
         <v>20</v>
       </c>
       <c r="L12" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M12" s="22"/>
       <c r="N12" s="6" t="s">
@@ -2772,7 +2769,7 @@
         <v>306</v>
       </c>
       <c r="T12" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="U12" s="61" t="s">
         <v>307</v>
@@ -2780,7 +2777,7 @@
       <c r="W12" s="16"/>
       <c r="X12" s="16"/>
     </row>
-    <row r="13" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -2798,7 +2795,7 @@
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H13" s="11">
         <v>11</v>
@@ -2813,7 +2810,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>117</v>
@@ -2832,7 +2829,7 @@
         <v>302</v>
       </c>
       <c r="S13" s="64" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="T13" s="67" t="s">
         <v>308</v>
@@ -2843,7 +2840,7 @@
       <c r="W13" s="16"/>
       <c r="X13" s="16"/>
     </row>
-    <row r="14" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -2870,13 +2867,13 @@
         <v>20</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K14" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L14" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M14" s="22" t="s">
         <v>60</v>
@@ -2898,7 +2895,7 @@
         <v>298</v>
       </c>
       <c r="T14" s="63" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="U14" s="61" t="s">
         <v>300</v>
@@ -2906,7 +2903,7 @@
       <c r="W14" s="16"/>
       <c r="X14" s="16"/>
     </row>
-    <row r="15" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -2939,7 +2936,7 @@
         <v>20</v>
       </c>
       <c r="L15" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M15" s="22" t="s">
         <v>60</v>
@@ -2961,7 +2958,7 @@
         <v>298</v>
       </c>
       <c r="T15" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="U15" s="61" t="s">
         <v>300</v>
@@ -2969,7 +2966,7 @@
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
     </row>
-    <row r="16" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -2987,7 +2984,7 @@
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H16" s="19">
         <v>14</v>
@@ -2996,13 +2993,13 @@
         <v>20</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M16" s="22"/>
       <c r="N16" s="6" t="s">
@@ -3024,7 +3021,7 @@
         <v>306</v>
       </c>
       <c r="T16" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U16" s="61" t="s">
         <v>307</v>
@@ -3032,7 +3029,7 @@
       <c r="W16" s="16"/>
       <c r="X16" s="16"/>
     </row>
-    <row r="17" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -3048,7 +3045,7 @@
       <c r="E17" s="30"/>
       <c r="F17" s="18"/>
       <c r="G17" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H17" s="11">
         <v>15</v>
@@ -3063,7 +3060,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M17" s="22" t="s">
         <v>55</v>
@@ -3085,7 +3082,7 @@
         <v>298</v>
       </c>
       <c r="T17" s="63" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="U17" s="61" t="s">
         <v>300</v>
@@ -3093,7 +3090,7 @@
       <c r="W17" s="16"/>
       <c r="X17" s="16"/>
     </row>
-    <row r="18" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
@@ -3111,7 +3108,7 @@
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H18" s="19">
         <v>16</v>
@@ -3126,7 +3123,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M18" s="22"/>
       <c r="N18" s="6" t="s">
@@ -3148,7 +3145,7 @@
         <v>306</v>
       </c>
       <c r="T18" s="63" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="U18" s="61" t="s">
         <v>307</v>
@@ -3156,7 +3153,7 @@
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
@@ -3174,7 +3171,7 @@
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H19" s="11">
         <v>17</v>
@@ -3189,7 +3186,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M19" s="22"/>
       <c r="N19" s="6" t="s">
@@ -3211,7 +3208,7 @@
         <v>306</v>
       </c>
       <c r="T19" s="63" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="U19" s="61" t="s">
         <v>307</v>
@@ -3219,7 +3216,7 @@
       <c r="W19" s="16"/>
       <c r="X19" s="16"/>
     </row>
-    <row r="20" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
@@ -3252,7 +3249,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M20" s="22"/>
       <c r="N20" s="6" t="s">
@@ -3274,7 +3271,7 @@
         <v>306</v>
       </c>
       <c r="T20" s="63" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="U20" s="61" t="s">
         <v>307</v>
@@ -3282,7 +3279,7 @@
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
     </row>
-    <row r="21" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
@@ -3315,7 +3312,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M21" s="22"/>
       <c r="N21" s="6" t="s">
@@ -3337,7 +3334,7 @@
         <v>306</v>
       </c>
       <c r="T21" s="63" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="U21" s="61" t="s">
         <v>307</v>
@@ -3345,7 +3342,7 @@
       <c r="W21" s="16"/>
       <c r="X21" s="16"/>
     </row>
-    <row r="22" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -3363,7 +3360,7 @@
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H22" s="11">
         <v>20</v>
@@ -3372,13 +3369,13 @@
         <v>19</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K22" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L22" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M22" s="22" t="s">
         <v>64</v>
@@ -3400,7 +3397,7 @@
         <v>298</v>
       </c>
       <c r="T22" s="63" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="U22" s="61" t="s">
         <v>300</v>
@@ -3408,7 +3405,7 @@
       <c r="W22" s="16"/>
       <c r="X22" s="16"/>
     </row>
-    <row r="23" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
@@ -3441,7 +3438,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M23" s="22"/>
       <c r="N23" s="6" t="s">
@@ -3463,7 +3460,7 @@
         <v>306</v>
       </c>
       <c r="T23" s="63" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="U23" s="61" t="s">
         <v>307</v>
@@ -3471,7 +3468,7 @@
       <c r="W23" s="16"/>
       <c r="X23" s="16"/>
     </row>
-    <row r="24" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>15</v>
       </c>
@@ -3504,7 +3501,7 @@
         <v>19</v>
       </c>
       <c r="L24" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M24" s="22"/>
       <c r="N24" s="6"/>
@@ -3518,21 +3515,21 @@
         <v>8</v>
       </c>
       <c r="R24" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S24" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T24" s="66" t="s">
         <v>162</v>
       </c>
       <c r="U24" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W24" s="16"/>
       <c r="X24" s="16"/>
     </row>
-    <row r="25" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>15</v>
       </c>
@@ -3550,7 +3547,7 @@
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H25" s="11">
         <v>23</v>
@@ -3559,18 +3556,18 @@
         <v>20</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>19</v>
       </c>
       <c r="L25" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M25" s="22"/>
       <c r="N25" s="6"/>
       <c r="O25" s="23" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P25" s="52" t="s">
         <v>19</v>
@@ -3579,21 +3576,21 @@
         <v>8</v>
       </c>
       <c r="R25" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S25" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T25" s="66" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="U25" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W25" s="16"/>
       <c r="X25" s="16"/>
     </row>
-    <row r="26" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>15</v>
       </c>
@@ -3626,7 +3623,7 @@
         <v>19</v>
       </c>
       <c r="L26" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M26" s="22"/>
       <c r="N26" s="6" t="s">
@@ -3642,21 +3639,21 @@
         <v>8</v>
       </c>
       <c r="R26" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S26" s="64" t="s">
+        <v>321</v>
+      </c>
+      <c r="T26" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="T26" s="66" t="s">
+      <c r="U26" s="64" t="s">
         <v>323</v>
-      </c>
-      <c r="U26" s="64" t="s">
-        <v>324</v>
       </c>
       <c r="W26" s="16"/>
       <c r="X26" s="16"/>
     </row>
-    <row r="27" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
@@ -3687,7 +3684,7 @@
         <v>20</v>
       </c>
       <c r="L27" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M27" s="22" t="s">
         <v>60</v>
@@ -3709,7 +3706,7 @@
         <v>298</v>
       </c>
       <c r="T27" s="63" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="U27" s="61" t="s">
         <v>300</v>
@@ -3717,7 +3714,7 @@
       <c r="W27" s="16"/>
       <c r="X27" s="16"/>
     </row>
-    <row r="28" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
@@ -3733,7 +3730,7 @@
       <c r="E28" s="30"/>
       <c r="F28" s="18"/>
       <c r="G28" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H28" s="19">
         <v>26</v>
@@ -3742,7 +3739,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K28" s="29" t="s">
         <v>19</v>
@@ -3756,21 +3753,21 @@
         <v>8</v>
       </c>
       <c r="R28" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S28" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T28" s="66" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="U28" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W28" s="16"/>
       <c r="X28" s="16"/>
     </row>
-    <row r="29" spans="1:24" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>15</v>
       </c>
@@ -3803,7 +3800,7 @@
         <v>19</v>
       </c>
       <c r="L29" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M29" s="22"/>
       <c r="N29" s="6"/>
@@ -3817,21 +3814,21 @@
         <v>8</v>
       </c>
       <c r="R29" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S29" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T29" s="66" t="s">
         <v>165</v>
       </c>
       <c r="U29" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W29" s="16"/>
       <c r="X29" s="16"/>
     </row>
-    <row r="30" spans="1:24" s="42" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" s="42" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>15</v>
       </c>
@@ -3864,7 +3861,7 @@
         <v>19</v>
       </c>
       <c r="L30" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M30" s="22"/>
       <c r="N30" s="22"/>
@@ -3874,8 +3871,8 @@
       <c r="P30" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="61" t="s">
-        <v>310</v>
+      <c r="Q30" s="61">
+        <v>6</v>
       </c>
       <c r="R30" s="62" t="s">
         <v>302</v>
@@ -3884,7 +3881,7 @@
         <v>303</v>
       </c>
       <c r="T30" s="63" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U30" s="61" t="s">
         <v>304</v>
@@ -3892,7 +3889,7 @@
       <c r="W30" s="43"/>
       <c r="X30" s="43"/>
     </row>
-    <row r="31" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>15</v>
       </c>
@@ -3908,7 +3905,7 @@
       <c r="E31" s="30"/>
       <c r="F31" s="18"/>
       <c r="G31" s="24" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H31" s="11">
         <v>29</v>
@@ -3917,7 +3914,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K31" s="29" t="s">
         <v>19</v>
@@ -3931,21 +3928,21 @@
         <v>8</v>
       </c>
       <c r="R31" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S31" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T31" s="66" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="U31" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W31" s="43"/>
       <c r="X31" s="43"/>
     </row>
-    <row r="32" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>15</v>
       </c>
@@ -3961,7 +3958,7 @@
       <c r="E32" s="30"/>
       <c r="F32" s="18"/>
       <c r="G32" s="24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H32" s="11">
         <v>30</v>
@@ -3970,7 +3967,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K32" s="29" t="s">
         <v>19</v>
@@ -3984,21 +3981,21 @@
         <v>8</v>
       </c>
       <c r="R32" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S32" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T32" s="66" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="U32" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W32" s="43"/>
       <c r="X32" s="43"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>15</v>
       </c>
@@ -4031,7 +4028,7 @@
         <v>19</v>
       </c>
       <c r="L33" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M33" s="22"/>
       <c r="N33" s="22" t="s">
@@ -4047,21 +4044,21 @@
         <v>8</v>
       </c>
       <c r="R33" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S33" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T33" s="66" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="U33" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W33" s="16"/>
       <c r="X33" s="16"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>15</v>
       </c>
@@ -4072,7 +4069,7 @@
         <v>127</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E34" s="30"/>
       <c r="F34" s="18"/>
@@ -4092,7 +4089,7 @@
         <v>19</v>
       </c>
       <c r="L34" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
@@ -4106,21 +4103,21 @@
         <v>8</v>
       </c>
       <c r="R34" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S34" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T34" s="66" t="s">
         <v>168</v>
       </c>
       <c r="U34" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W34" s="16"/>
       <c r="X34" s="16"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>15</v>
       </c>
@@ -4131,7 +4128,7 @@
         <v>127</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E35" s="30"/>
       <c r="F35" s="18"/>
@@ -4151,7 +4148,7 @@
         <v>20</v>
       </c>
       <c r="L35" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
@@ -4165,21 +4162,21 @@
         <v>8</v>
       </c>
       <c r="R35" s="69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S35" s="68" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T35" s="70" t="s">
         <v>169</v>
       </c>
       <c r="U35" s="68" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W35" s="16"/>
       <c r="X35" s="16"/>
     </row>
-    <row r="36" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>15</v>
       </c>
@@ -4190,7 +4187,7 @@
         <v>127</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E36" s="30" t="s">
         <v>146</v>
@@ -4212,7 +4209,7 @@
         <v>20</v>
       </c>
       <c r="L36" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M36" s="22" t="s">
         <v>58</v>
@@ -4234,7 +4231,7 @@
         <v>298</v>
       </c>
       <c r="T36" s="63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="U36" s="61" t="s">
         <v>300</v>
@@ -4242,7 +4239,7 @@
       <c r="W36" s="43"/>
       <c r="X36" s="43"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>15</v>
       </c>
@@ -4253,7 +4250,7 @@
         <v>127</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E37" s="30" t="s">
         <v>146</v>
@@ -4275,7 +4272,7 @@
         <v>19</v>
       </c>
       <c r="L37" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
@@ -4289,21 +4286,21 @@
         <v>8</v>
       </c>
       <c r="R37" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S37" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T37" s="66" t="s">
         <v>171</v>
       </c>
       <c r="U37" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W37" s="16"/>
       <c r="X37" s="16"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>15</v>
       </c>
@@ -4314,14 +4311,14 @@
         <v>127</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E38" s="30" t="s">
         <v>146</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H38" s="19">
         <v>36</v>
@@ -4330,7 +4327,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K38" s="29" t="s">
         <v>19</v>
@@ -4344,21 +4341,21 @@
         <v>8</v>
       </c>
       <c r="R38" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S38" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T38" s="66" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="U38" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W38" s="16"/>
       <c r="X38" s="16"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>15</v>
       </c>
@@ -4369,14 +4366,14 @@
         <v>127</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E39" s="30" t="s">
         <v>146</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H39" s="11">
         <v>37</v>
@@ -4385,7 +4382,7 @@
         <v>20</v>
       </c>
       <c r="J39" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K39" s="29" t="s">
         <v>19</v>
@@ -4399,21 +4396,21 @@
         <v>8</v>
       </c>
       <c r="R39" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S39" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T39" s="66" t="s">
         <v>169</v>
       </c>
       <c r="U39" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W39" s="16"/>
       <c r="X39" s="16"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>15</v>
       </c>
@@ -4424,14 +4421,14 @@
         <v>127</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E40" s="30" t="s">
         <v>146</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="24" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H40" s="19">
         <v>38</v>
@@ -4440,7 +4437,7 @@
         <v>20</v>
       </c>
       <c r="J40" s="27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K40" s="29" t="s">
         <v>19</v>
@@ -4454,21 +4451,21 @@
         <v>8</v>
       </c>
       <c r="R40" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S40" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T40" s="66" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="U40" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W40" s="16"/>
       <c r="X40" s="16"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>15</v>
       </c>
@@ -4479,14 +4476,14 @@
         <v>127</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E41" s="30" t="s">
         <v>146</v>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H41" s="11">
         <v>39</v>
@@ -4495,7 +4492,7 @@
         <v>20</v>
       </c>
       <c r="J41" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K41" s="29" t="s">
         <v>19</v>
@@ -4509,21 +4506,21 @@
         <v>8</v>
       </c>
       <c r="R41" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S41" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T41" s="66" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U41" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W41" s="16"/>
       <c r="X41" s="16"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>15</v>
       </c>
@@ -4534,14 +4531,14 @@
         <v>127</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E42" s="30" t="s">
         <v>125</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H42" s="11">
         <v>40</v>
@@ -4556,7 +4553,7 @@
         <v>19</v>
       </c>
       <c r="L42" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
@@ -4570,21 +4567,21 @@
         <v>8</v>
       </c>
       <c r="R42" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S42" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T42" s="66" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="U42" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W42" s="16"/>
       <c r="X42" s="16"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>15</v>
       </c>
@@ -4615,7 +4612,7 @@
         <v>19</v>
       </c>
       <c r="L43" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
@@ -4629,21 +4626,21 @@
         <v>8</v>
       </c>
       <c r="R43" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S43" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T43" s="66" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="U43" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W43" s="16"/>
       <c r="X43" s="16"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>15</v>
       </c>
@@ -4674,7 +4671,7 @@
         <v>19</v>
       </c>
       <c r="L44" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
@@ -4688,21 +4685,21 @@
         <v>8</v>
       </c>
       <c r="R44" s="65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S44" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T44" s="66" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="U44" s="64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W44" s="16"/>
       <c r="X44" s="16"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>15</v>
       </c>
@@ -4733,7 +4730,7 @@
         <v>20</v>
       </c>
       <c r="L45" s="51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
@@ -4749,7 +4746,7 @@
       <c r="W45" s="16"/>
       <c r="X45" s="16"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>15</v>
       </c>
@@ -4780,7 +4777,7 @@
         <v>20</v>
       </c>
       <c r="L46" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M46" s="22"/>
       <c r="N46" s="22" t="s">
@@ -4802,7 +4799,7 @@
         <v>306</v>
       </c>
       <c r="T46" s="63" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="U46" s="61" t="s">
         <v>307</v>
@@ -4810,7 +4807,7 @@
       <c r="W46" s="16"/>
       <c r="X46" s="16"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>15</v>
       </c>
@@ -4833,7 +4830,7 @@
         <v>20</v>
       </c>
       <c r="J47" s="35" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K47" s="29" t="s">
         <v>19</v>
@@ -4855,7 +4852,7 @@
         <v>306</v>
       </c>
       <c r="T47" s="63" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="U47" s="61" t="s">
         <v>307</v>
@@ -4863,7 +4860,7 @@
       <c r="W47" s="36"/>
       <c r="X47" s="36"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
@@ -4884,19 +4881,19 @@
         <v>8</v>
       </c>
       <c r="R48" s="69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S48" s="68" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T48" s="70" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="U48" s="68" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="8"/>
       <c r="C49" s="9"/>
@@ -4919,7 +4916,7 @@
       <c r="T49" s="46"/>
       <c r="U49" s="44"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
@@ -4942,7 +4939,7 @@
       <c r="T50" s="46"/>
       <c r="U50" s="44"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9"/>
@@ -4965,7 +4962,7 @@
       <c r="T51" s="46"/>
       <c r="U51" s="44"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9"/>
@@ -4988,7 +4985,7 @@
       <c r="T52" s="46"/>
       <c r="U52" s="44"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="8"/>
       <c r="C53" s="9"/>
@@ -5011,7 +5008,7 @@
       <c r="T53" s="46"/>
       <c r="U53" s="44"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="38"/>
       <c r="B54" s="33"/>
       <c r="C54" s="39"/>
@@ -5034,7 +5031,7 @@
       <c r="T54" s="46"/>
       <c r="U54" s="44"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="38"/>
       <c r="B55" s="33"/>
       <c r="C55" s="39"/>
@@ -5057,7 +5054,7 @@
       <c r="T55" s="46"/>
       <c r="U55" s="44"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="38"/>
       <c r="B56" s="33"/>
       <c r="C56" s="39"/>
@@ -5080,7 +5077,7 @@
       <c r="T56" s="46"/>
       <c r="U56" s="44"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="38"/>
       <c r="B57" s="33"/>
       <c r="C57" s="39"/>
@@ -5103,7 +5100,7 @@
       <c r="T57" s="46"/>
       <c r="U57" s="44"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="38"/>
       <c r="B58" s="33"/>
       <c r="C58" s="39"/>
@@ -5126,7 +5123,7 @@
       <c r="T58" s="46"/>
       <c r="U58" s="44"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="38"/>
       <c r="B59" s="33"/>
       <c r="C59" s="39"/>
@@ -5149,7 +5146,7 @@
       <c r="T59" s="46"/>
       <c r="U59" s="44"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="38"/>
       <c r="B60" s="33"/>
       <c r="C60" s="39"/>
@@ -5172,7 +5169,7 @@
       <c r="T60" s="46"/>
       <c r="U60" s="44"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="38"/>
       <c r="B61" s="33"/>
       <c r="C61" s="39"/>
@@ -5195,7 +5192,7 @@
       <c r="T61" s="46"/>
       <c r="U61" s="44"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="38"/>
       <c r="B62" s="33"/>
       <c r="C62" s="39"/>
@@ -5218,7 +5215,7 @@
       <c r="T62" s="46"/>
       <c r="U62" s="44"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="38"/>
       <c r="B63" s="33"/>
       <c r="C63" s="39"/>
@@ -5241,7 +5238,7 @@
       <c r="T63" s="46"/>
       <c r="U63" s="44"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="38"/>
       <c r="B64" s="33"/>
       <c r="C64" s="39"/>
@@ -5264,7 +5261,7 @@
       <c r="T64" s="46"/>
       <c r="U64" s="44"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="38"/>
       <c r="B65" s="33"/>
       <c r="C65" s="39"/>
@@ -5287,7 +5284,7 @@
       <c r="T65" s="46"/>
       <c r="U65" s="44"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="38"/>
       <c r="B66" s="33"/>
       <c r="C66" s="39"/>
@@ -5310,7 +5307,7 @@
       <c r="T66" s="46"/>
       <c r="U66" s="44"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="38"/>
       <c r="B67" s="33"/>
       <c r="C67" s="39"/>
@@ -5333,7 +5330,7 @@
       <c r="T67" s="46"/>
       <c r="U67" s="44"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="38"/>
       <c r="B68" s="33"/>
       <c r="C68" s="39"/>
@@ -5356,7 +5353,7 @@
       <c r="T68" s="46"/>
       <c r="U68" s="44"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="38"/>
       <c r="B69" s="33"/>
       <c r="C69" s="39"/>
@@ -5379,7 +5376,7 @@
       <c r="T69" s="46"/>
       <c r="U69" s="44"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="38"/>
       <c r="B70" s="33"/>
       <c r="C70" s="39"/>
@@ -5402,7 +5399,7 @@
       <c r="T70" s="46"/>
       <c r="U70" s="44"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="38"/>
       <c r="B71" s="33"/>
       <c r="C71" s="39"/>
@@ -5425,7 +5422,7 @@
       <c r="T71" s="46"/>
       <c r="U71" s="44"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="38"/>
       <c r="B72" s="33"/>
       <c r="C72" s="39"/>
@@ -5448,7 +5445,7 @@
       <c r="T72" s="46"/>
       <c r="U72" s="44"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="38"/>
       <c r="B73" s="33"/>
       <c r="C73" s="39"/>
@@ -5471,7 +5468,7 @@
       <c r="T73" s="46"/>
       <c r="U73" s="44"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="38"/>
       <c r="B74" s="33"/>
       <c r="C74" s="39"/>
@@ -5494,7 +5491,7 @@
       <c r="T74" s="46"/>
       <c r="U74" s="44"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="38"/>
       <c r="B75" s="33"/>
       <c r="C75" s="39"/>
@@ -5517,7 +5514,7 @@
       <c r="T75" s="46"/>
       <c r="U75" s="44"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" s="38"/>
       <c r="B76" s="33"/>
       <c r="C76" s="39"/>
@@ -5540,813 +5537,813 @@
       <c r="T76" s="46"/>
       <c r="U76" s="44"/>
     </row>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="129" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="130" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="131" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="132" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="133" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="134" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="135" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="136" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="137" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="138" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="139" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="140" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="141" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="142" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="143" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="144" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="214" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="215" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="216" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="217" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="218" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="219" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="220" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="221" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="222" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="223" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="224" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="225" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="226" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="227" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="228" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="229" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="230" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="231" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="232" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="233" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="234" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="235" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="236" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="237" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="238" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="239" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="240" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="241" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="242" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="243" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="244" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="245" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="246" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="247" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="248" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="249" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="250" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="251" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="252" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="253" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="254" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="255" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="256" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="257" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="258" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="259" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="260" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="261" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="262" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="263" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="264" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="265" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="266" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="267" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="268" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="269" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="270" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="271" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="272" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="273" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="274" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="275" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="276" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="277" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="278" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="279" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="280" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="281" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="282" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="283" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="285" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="286" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="287" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="288" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="289" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="290" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="129" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="130" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="131" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="132" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="133" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="134" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="135" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="136" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="137" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="138" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="139" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="140" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="141" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="142" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="143" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="144" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="289" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="290" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="34" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="34" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="34" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="34" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" s="34" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" s="34" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" s="34" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" s="34" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" s="34" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" s="34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" s="34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" s="34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" s="34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" s="34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" s="34" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" s="34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" s="34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" s="34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" s="34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" s="34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" s="34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" s="34" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" s="34" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" s="34" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" s="34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" s="34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" s="34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" s="34" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" s="34" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" s="34" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" s="34" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" s="34" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" s="34" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" s="34" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" s="34" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" s="34" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" s="34" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" s="34" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="34" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" s="34" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" s="34" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="34" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" s="34" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" s="34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" s="34" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" s="34" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" s="34" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" s="34" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" s="34" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" s="34" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" s="34" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" s="34" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" s="34" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" s="34" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" s="34" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" s="34" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" s="34" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" s="34" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" s="34" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" s="34" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" s="34" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" s="34" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" s="34" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="34" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" s="34" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" s="34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" s="34" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A369" s="34" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A370" s="34" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A371" s="34" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A372" s="34" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A373" s="34" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A374" s="34" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A375" s="34" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A376" s="34" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A377" s="34" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A378" s="34" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A379" s="34" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A380" s="34" t="s">
         <v>296</v>
       </c>
@@ -6356,6 +6353,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -6370,12 +6373,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W43:W46">
@@ -6449,27 +6446,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" style="1"/>
-    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -6486,7 +6483,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -6510,7 +6507,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -6529,7 +6526,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -6548,7 +6545,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -6564,7 +6561,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -6581,7 +6578,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -6598,7 +6595,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -6613,7 +6610,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -6628,7 +6625,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -6643,7 +6640,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -6658,7 +6655,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -6673,7 +6670,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -6688,7 +6685,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -6703,7 +6700,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -6718,7 +6715,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -6733,7 +6730,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -6747,7 +6744,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -6761,7 +6758,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -6775,7 +6772,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -6789,7 +6786,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -6804,7 +6801,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6819,7 +6816,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -6834,7 +6831,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -6849,7 +6846,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -6864,7 +6861,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -6879,7 +6876,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -6894,7 +6891,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6909,7 +6906,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -6924,7 +6921,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -6939,7 +6936,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -6954,7 +6951,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -6969,7 +6966,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -6984,7 +6981,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -6999,7 +6996,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -7014,7 +7011,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -7029,7 +7026,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -7044,7 +7041,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -7059,7 +7056,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -7074,7 +7071,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -7089,7 +7086,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -7104,7 +7101,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -7119,7 +7116,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -7134,7 +7131,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -7149,7 +7146,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -7164,7 +7161,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -7179,7 +7176,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -7194,7 +7191,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -7209,7 +7206,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -7221,7 +7218,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -7233,7 +7230,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -7246,7 +7243,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -7259,7 +7256,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -7272,7 +7269,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -7285,7 +7282,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -7298,7 +7295,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -7311,7 +7308,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -7324,7 +7321,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -7337,7 +7334,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -7350,7 +7347,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -7363,7 +7360,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -7376,7 +7373,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -7389,7 +7386,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -7402,7 +7399,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -7415,7 +7412,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -7428,7 +7425,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -7441,7 +7438,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -7454,7 +7451,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -7467,7 +7464,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -7480,7 +7477,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -7493,7 +7490,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -7507,7 +7504,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -7521,7 +7518,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -7535,7 +7532,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -7549,7 +7546,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -7563,7 +7560,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -7577,7 +7574,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -7591,7 +7588,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -7605,7 +7602,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -7619,7 +7616,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -7633,7 +7630,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -7647,7 +7644,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -7661,7 +7658,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -7675,7 +7672,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -7689,7 +7686,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -7703,7 +7700,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -7717,7 +7714,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -7731,7 +7728,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -7745,7 +7742,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -7759,7 +7756,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -7773,7 +7770,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -7787,7 +7784,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -7801,7 +7798,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -7815,7 +7812,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -7829,7 +7826,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -7843,7 +7840,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -7857,7 +7854,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -7871,7 +7868,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -7885,7 +7882,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -7899,7 +7896,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -7913,7 +7910,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -7927,7 +7924,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -7941,7 +7938,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -7955,7 +7952,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -7969,7 +7966,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -7983,7 +7980,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -7997,7 +7994,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -8011,7 +8008,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -8025,7 +8022,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -8039,7 +8036,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -8053,7 +8050,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -8067,7 +8064,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -8081,7 +8078,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -8095,7 +8092,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -8109,7 +8106,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -8123,7 +8120,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -8137,7 +8134,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -8151,7 +8148,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -8165,7 +8162,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -8179,7 +8176,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -8193,7 +8190,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -8207,7 +8204,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -8221,7 +8218,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -8235,7 +8232,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -8249,7 +8246,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -8263,7 +8260,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -8277,7 +8274,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -8291,7 +8288,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -8305,7 +8302,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -8319,7 +8316,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -8333,7 +8330,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -8347,7 +8344,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -8361,7 +8358,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>

</xml_diff>

<commit_message>
Asignación de autores de recursos mat 7 tema 11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion11/ESCALETA MA_07_11_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion11/ESCALETA MA_07_11_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion11\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
@@ -13,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$P$1:$P$380</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="386">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1165,6 +1170,18 @@
   </si>
   <si>
     <t>Recurso M5A-07</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
+  </si>
+  <si>
+    <t>Sandra Ortiz</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
+  </si>
+  <si>
+    <t>Jennifer Rojas</t>
   </si>
 </sst>
 </file>
@@ -1653,13 +1670,22 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1705,15 +1731,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1776,7 +1793,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1811,7 +1828,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2021,11 +2038,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:X380"/>
+  <dimension ref="A1:X381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P5" sqref="P5:P46"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T381" sqref="T381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2056,94 +2073,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="79" t="s">
+      <c r="H1" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="I1" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="88" t="s">
+      <c r="K1" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="86" t="s">
+      <c r="L1" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="92" t="s">
+      <c r="M1" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="92"/>
-      <c r="O1" s="81" t="s">
+      <c r="N1" s="95"/>
+      <c r="O1" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="81" t="s">
+      <c r="P1" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="97" t="s">
+      <c r="Q1" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="99" t="s">
+      <c r="R1" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="97" t="s">
+      <c r="S1" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="98" t="s">
+      <c r="T1" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="97" t="s">
+      <c r="U1" s="80" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="87"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="90"/>
       <c r="M2" s="3" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="97"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="80"/>
     </row>
     <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -2516,6 +2533,9 @@
       <c r="U8" s="61" t="s">
         <v>300</v>
       </c>
+      <c r="V8" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="W8" s="16"/>
       <c r="X8" s="16"/>
     </row>
@@ -2579,6 +2599,9 @@
       <c r="U9" s="61" t="s">
         <v>306</v>
       </c>
+      <c r="V9" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="W9" s="16"/>
       <c r="X9" s="16"/>
     </row>
@@ -2644,6 +2667,9 @@
       <c r="U10" s="61" t="s">
         <v>300</v>
       </c>
+      <c r="V10" s="4" t="s">
+        <v>383</v>
+      </c>
       <c r="W10" s="16"/>
       <c r="X10" s="16"/>
     </row>
@@ -2707,6 +2733,9 @@
       <c r="U11" s="61" t="s">
         <v>306</v>
       </c>
+      <c r="V11" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="W11" s="16"/>
       <c r="X11" s="16"/>
     </row>
@@ -2770,6 +2799,9 @@
       <c r="U12" s="61" t="s">
         <v>306</v>
       </c>
+      <c r="V12" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="W12" s="16"/>
       <c r="X12" s="16"/>
     </row>
@@ -2833,6 +2865,9 @@
       <c r="U13" s="64" t="s">
         <v>308</v>
       </c>
+      <c r="V13" s="4" t="s">
+        <v>383</v>
+      </c>
       <c r="W13" s="16"/>
       <c r="X13" s="16"/>
     </row>
@@ -2860,7 +2895,7 @@
         <v>12</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="27" t="s">
         <v>343</v>
@@ -2896,6 +2931,9 @@
       <c r="U14" s="61" t="s">
         <v>300</v>
       </c>
+      <c r="V14" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="W14" s="16"/>
       <c r="X14" s="16"/>
     </row>
@@ -2959,6 +2997,9 @@
       <c r="U15" s="61" t="s">
         <v>300</v>
       </c>
+      <c r="V15" s="4" t="s">
+        <v>385</v>
+      </c>
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
     </row>
@@ -3021,6 +3062,9 @@
       </c>
       <c r="U16" s="61" t="s">
         <v>306</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>384</v>
       </c>
       <c r="W16" s="16"/>
       <c r="X16" s="16"/>
@@ -3146,6 +3190,9 @@
       <c r="U18" s="61" t="s">
         <v>306</v>
       </c>
+      <c r="V18" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
     </row>
@@ -3209,6 +3256,9 @@
       <c r="U19" s="61" t="s">
         <v>306</v>
       </c>
+      <c r="V19" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="W19" s="16"/>
       <c r="X19" s="16"/>
     </row>
@@ -3272,6 +3322,9 @@
       <c r="U20" s="61" t="s">
         <v>306</v>
       </c>
+      <c r="V20" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
     </row>
@@ -3335,6 +3388,9 @@
       <c r="U21" s="61" t="s">
         <v>306</v>
       </c>
+      <c r="V21" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="W21" s="16"/>
       <c r="X21" s="16"/>
     </row>
@@ -3460,6 +3516,9 @@
       </c>
       <c r="U23" s="61" t="s">
         <v>306</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>384</v>
       </c>
       <c r="W23" s="16"/>
       <c r="X23" s="16"/>
@@ -3881,6 +3940,9 @@
       </c>
       <c r="U30" s="61" t="s">
         <v>306</v>
+      </c>
+      <c r="V30" s="42" t="s">
+        <v>385</v>
       </c>
       <c r="W30" s="43"/>
       <c r="X30" s="43"/>
@@ -4799,6 +4861,9 @@
       </c>
       <c r="U46" s="61" t="s">
         <v>306</v>
+      </c>
+      <c r="V46" s="4" t="s">
+        <v>385</v>
       </c>
       <c r="W46" s="16"/>
       <c r="X46" s="16"/>
@@ -6275,64 +6340,87 @@
         <v>284</v>
       </c>
     </row>
-    <row r="369" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" s="34" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="370" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370" s="34" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="371" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" s="34" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="372" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372" s="34" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="373" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" s="34" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="374" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" s="34" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="375" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" s="34" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="376" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" s="34" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="377" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" s="34" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="378" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" s="34" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="379" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" s="34" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="380" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" s="34" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="381" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D381" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="N381" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q381" s="61">
+        <v>6</v>
+      </c>
+      <c r="R381" s="62" t="s">
+        <v>302</v>
+      </c>
+      <c r="S381" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="T381" s="63" t="s">
+        <v>336</v>
+      </c>
+      <c r="V381" s="4" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -6344,12 +6432,6 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -6364,6 +6446,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W43:W46">
@@ -6397,7 +6485,7 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N30:N76</xm:sqref>
+          <xm:sqref>N30:N76 N381</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -6474,7 +6562,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -6517,7 +6605,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -6536,7 +6624,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -6552,7 +6640,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -6586,7 +6674,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -6601,7 +6689,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -6616,7 +6704,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -6631,7 +6719,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -6646,7 +6734,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -6661,7 +6749,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -6676,7 +6764,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -6691,7 +6779,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -6706,7 +6794,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -6721,7 +6809,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -6735,7 +6823,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -6749,7 +6837,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -6763,7 +6851,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -6777,7 +6865,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -6792,7 +6880,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6807,7 +6895,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -6822,7 +6910,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -6837,7 +6925,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -6852,7 +6940,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -6867,7 +6955,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -6882,7 +6970,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6897,7 +6985,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -6912,7 +7000,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -6927,7 +7015,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -6942,7 +7030,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -6957,7 +7045,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -6972,7 +7060,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -6987,7 +7075,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -7002,7 +7090,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -7017,7 +7105,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -7032,7 +7120,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -7047,7 +7135,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -7062,7 +7150,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -7077,7 +7165,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -7092,7 +7180,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -7107,7 +7195,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -7122,7 +7210,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -7137,7 +7225,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -7152,7 +7240,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -7167,7 +7255,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -7182,7 +7270,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -7197,7 +7285,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -7209,7 +7297,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -7221,7 +7309,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -7234,7 +7322,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -7247,7 +7335,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -7260,7 +7348,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>

</xml_diff>

<commit_message>
Asignación de autores Mat 7 tema 11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion11/ESCALETA MA_07_11_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion11/ESCALETA MA_07_11_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="389">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1188,6 +1188,9 @@
   </si>
   <si>
     <t>Johanna Montejo</t>
+  </si>
+  <si>
+    <t>Andrea Sabogal</t>
   </si>
 </sst>
 </file>
@@ -1676,13 +1679,22 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1728,15 +1740,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2043,12 +2046,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:X381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2079,94 +2081,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="79" t="s">
+      <c r="H1" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="I1" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="88" t="s">
+      <c r="K1" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="86" t="s">
+      <c r="L1" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="92" t="s">
+      <c r="M1" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="92"/>
-      <c r="O1" s="81" t="s">
+      <c r="N1" s="95"/>
+      <c r="O1" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="81" t="s">
+      <c r="P1" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="97" t="s">
+      <c r="Q1" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="99" t="s">
+      <c r="R1" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="97" t="s">
+      <c r="S1" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="98" t="s">
+      <c r="T1" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="97" t="s">
+      <c r="U1" s="80" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="87"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="90"/>
       <c r="M2" s="3" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="97"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="80"/>
     </row>
     <row r="3" spans="1:24" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -3009,7 +3011,7 @@
       <c r="U15" s="61" t="s">
         <v>300</v>
       </c>
-      <c r="V15" s="4" t="s">
+      <c r="V15" s="49" t="s">
         <v>385</v>
       </c>
       <c r="W15" s="16"/>
@@ -3081,7 +3083,7 @@
       <c r="W16" s="16"/>
       <c r="X16" s="16"/>
     </row>
-    <row r="17" spans="1:24" ht="14.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -3139,6 +3141,9 @@
       <c r="U17" s="61" t="s">
         <v>300</v>
       </c>
+      <c r="V17" s="49" t="s">
+        <v>385</v>
+      </c>
       <c r="W17" s="16"/>
       <c r="X17" s="16"/>
     </row>
@@ -3406,7 +3411,7 @@
       <c r="W21" s="16"/>
       <c r="X21" s="16"/>
     </row>
-    <row r="22" spans="1:24" ht="14.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -3465,6 +3470,9 @@
       </c>
       <c r="U22" s="61" t="s">
         <v>300</v>
+      </c>
+      <c r="V22" s="49" t="s">
+        <v>383</v>
       </c>
       <c r="W22" s="16"/>
       <c r="X22" s="16"/>
@@ -3720,7 +3728,7 @@
       <c r="W26" s="16"/>
       <c r="X26" s="16"/>
     </row>
-    <row r="27" spans="1:24" ht="14.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
@@ -3778,10 +3786,13 @@
       <c r="U27" s="61" t="s">
         <v>300</v>
       </c>
+      <c r="V27" s="49" t="s">
+        <v>388</v>
+      </c>
       <c r="W27" s="16"/>
       <c r="X27" s="16"/>
     </row>
-    <row r="28" spans="1:24" ht="14.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
@@ -3953,13 +3964,13 @@
       <c r="U30" s="61" t="s">
         <v>306</v>
       </c>
-      <c r="V30" s="42" t="s">
+      <c r="V30" s="49" t="s">
         <v>385</v>
       </c>
       <c r="W30" s="43"/>
       <c r="X30" s="43"/>
     </row>
-    <row r="31" spans="1:24" s="42" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>15</v>
       </c>
@@ -4012,7 +4023,7 @@
       <c r="W31" s="43"/>
       <c r="X31" s="43"/>
     </row>
-    <row r="32" spans="1:24" s="42" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>15</v>
       </c>
@@ -4128,7 +4139,7 @@
       <c r="W33" s="16"/>
       <c r="X33" s="16"/>
     </row>
-    <row r="34" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>15</v>
       </c>
@@ -4246,7 +4257,7 @@
       <c r="W35" s="16"/>
       <c r="X35" s="16"/>
     </row>
-    <row r="36" spans="1:24" s="42" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>15</v>
       </c>
@@ -4305,6 +4316,9 @@
       </c>
       <c r="U36" s="61" t="s">
         <v>300</v>
+      </c>
+      <c r="V36" s="49" t="s">
+        <v>386</v>
       </c>
       <c r="W36" s="43"/>
       <c r="X36" s="43"/>
@@ -4370,7 +4384,7 @@
       <c r="W37" s="16"/>
       <c r="X37" s="16"/>
     </row>
-    <row r="38" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>15</v>
       </c>
@@ -4425,7 +4439,7 @@
       <c r="W38" s="16"/>
       <c r="X38" s="16"/>
     </row>
-    <row r="39" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>15</v>
       </c>
@@ -4480,7 +4494,7 @@
       <c r="W39" s="16"/>
       <c r="X39" s="16"/>
     </row>
-    <row r="40" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>15</v>
       </c>
@@ -4535,7 +4549,7 @@
       <c r="W40" s="16"/>
       <c r="X40" s="16"/>
     </row>
-    <row r="41" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>15</v>
       </c>
@@ -4769,7 +4783,7 @@
       <c r="W44" s="16"/>
       <c r="X44" s="16"/>
     </row>
-    <row r="45" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>15</v>
       </c>
@@ -4874,13 +4888,13 @@
       <c r="U46" s="61" t="s">
         <v>306</v>
       </c>
-      <c r="V46" s="4" t="s">
+      <c r="V46" s="49" t="s">
         <v>385</v>
       </c>
       <c r="W46" s="16"/>
       <c r="X46" s="16"/>
     </row>
-    <row r="47" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>15</v>
       </c>
@@ -4930,10 +4944,13 @@
       <c r="U47" s="61" t="s">
         <v>306</v>
       </c>
+      <c r="V47" s="49" t="s">
+        <v>388</v>
+      </c>
       <c r="W47" s="36"/>
       <c r="X47" s="36"/>
     </row>
-    <row r="48" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
@@ -4956,7 +4973,7 @@
       <c r="T48" s="70"/>
       <c r="U48" s="68"/>
     </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="8"/>
       <c r="C49" s="9"/>
@@ -4979,7 +4996,7 @@
       <c r="T49" s="46"/>
       <c r="U49" s="44"/>
     </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
@@ -5002,7 +5019,7 @@
       <c r="T50" s="46"/>
       <c r="U50" s="44"/>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9"/>
@@ -5025,7 +5042,7 @@
       <c r="T51" s="46"/>
       <c r="U51" s="44"/>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9"/>
@@ -5048,7 +5065,7 @@
       <c r="T52" s="46"/>
       <c r="U52" s="44"/>
     </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="8"/>
       <c r="C53" s="9"/>
@@ -5071,7 +5088,7 @@
       <c r="T53" s="46"/>
       <c r="U53" s="44"/>
     </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="38"/>
       <c r="B54" s="33"/>
       <c r="C54" s="39"/>
@@ -5094,7 +5111,7 @@
       <c r="T54" s="46"/>
       <c r="U54" s="44"/>
     </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="38"/>
       <c r="B55" s="33"/>
       <c r="C55" s="39"/>
@@ -5117,7 +5134,7 @@
       <c r="T55" s="46"/>
       <c r="U55" s="44"/>
     </row>
-    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="38"/>
       <c r="B56" s="33"/>
       <c r="C56" s="39"/>
@@ -5140,7 +5157,7 @@
       <c r="T56" s="46"/>
       <c r="U56" s="44"/>
     </row>
-    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="38"/>
       <c r="B57" s="33"/>
       <c r="C57" s="39"/>
@@ -5163,7 +5180,7 @@
       <c r="T57" s="46"/>
       <c r="U57" s="44"/>
     </row>
-    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="38"/>
       <c r="B58" s="33"/>
       <c r="C58" s="39"/>
@@ -5186,7 +5203,7 @@
       <c r="T58" s="46"/>
       <c r="U58" s="44"/>
     </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="38"/>
       <c r="B59" s="33"/>
       <c r="C59" s="39"/>
@@ -5209,7 +5226,7 @@
       <c r="T59" s="46"/>
       <c r="U59" s="44"/>
     </row>
-    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="38"/>
       <c r="B60" s="33"/>
       <c r="C60" s="39"/>
@@ -5232,7 +5249,7 @@
       <c r="T60" s="46"/>
       <c r="U60" s="44"/>
     </row>
-    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="38"/>
       <c r="B61" s="33"/>
       <c r="C61" s="39"/>
@@ -5255,7 +5272,7 @@
       <c r="T61" s="46"/>
       <c r="U61" s="44"/>
     </row>
-    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="38"/>
       <c r="B62" s="33"/>
       <c r="C62" s="39"/>
@@ -5278,7 +5295,7 @@
       <c r="T62" s="46"/>
       <c r="U62" s="44"/>
     </row>
-    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="38"/>
       <c r="B63" s="33"/>
       <c r="C63" s="39"/>
@@ -5301,7 +5318,7 @@
       <c r="T63" s="46"/>
       <c r="U63" s="44"/>
     </row>
-    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="38"/>
       <c r="B64" s="33"/>
       <c r="C64" s="39"/>
@@ -5324,7 +5341,7 @@
       <c r="T64" s="46"/>
       <c r="U64" s="44"/>
     </row>
-    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="38"/>
       <c r="B65" s="33"/>
       <c r="C65" s="39"/>
@@ -5347,7 +5364,7 @@
       <c r="T65" s="46"/>
       <c r="U65" s="44"/>
     </row>
-    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="38"/>
       <c r="B66" s="33"/>
       <c r="C66" s="39"/>
@@ -5370,7 +5387,7 @@
       <c r="T66" s="46"/>
       <c r="U66" s="44"/>
     </row>
-    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="38"/>
       <c r="B67" s="33"/>
       <c r="C67" s="39"/>
@@ -5393,7 +5410,7 @@
       <c r="T67" s="46"/>
       <c r="U67" s="44"/>
     </row>
-    <row r="68" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="38"/>
       <c r="B68" s="33"/>
       <c r="C68" s="39"/>
@@ -5416,7 +5433,7 @@
       <c r="T68" s="46"/>
       <c r="U68" s="44"/>
     </row>
-    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="38"/>
       <c r="B69" s="33"/>
       <c r="C69" s="39"/>
@@ -5439,7 +5456,7 @@
       <c r="T69" s="46"/>
       <c r="U69" s="44"/>
     </row>
-    <row r="70" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="38"/>
       <c r="B70" s="33"/>
       <c r="C70" s="39"/>
@@ -5462,7 +5479,7 @@
       <c r="T70" s="46"/>
       <c r="U70" s="44"/>
     </row>
-    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="38"/>
       <c r="B71" s="33"/>
       <c r="C71" s="39"/>
@@ -5485,7 +5502,7 @@
       <c r="T71" s="46"/>
       <c r="U71" s="44"/>
     </row>
-    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="38"/>
       <c r="B72" s="33"/>
       <c r="C72" s="39"/>
@@ -5508,7 +5525,7 @@
       <c r="T72" s="46"/>
       <c r="U72" s="44"/>
     </row>
-    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="38"/>
       <c r="B73" s="33"/>
       <c r="C73" s="39"/>
@@ -5531,7 +5548,7 @@
       <c r="T73" s="46"/>
       <c r="U73" s="44"/>
     </row>
-    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="38"/>
       <c r="B74" s="33"/>
       <c r="C74" s="39"/>
@@ -5554,7 +5571,7 @@
       <c r="T74" s="46"/>
       <c r="U74" s="44"/>
     </row>
-    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="38"/>
       <c r="B75" s="33"/>
       <c r="C75" s="39"/>
@@ -5577,7 +5594,7 @@
       <c r="T75" s="46"/>
       <c r="U75" s="44"/>
     </row>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" s="38"/>
       <c r="B76" s="33"/>
       <c r="C76" s="39"/>
@@ -5600,814 +5617,637 @@
       <c r="T76" s="46"/>
       <c r="U76" s="44"/>
     </row>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="129" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="130" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="131" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="132" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="133" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="134" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="135" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="136" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="137" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="138" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="139" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="140" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="141" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="142" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="143" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="144" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="214" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="215" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="216" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="217" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="218" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="219" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="220" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="221" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="222" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="223" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="224" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="225" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="226" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="227" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="228" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="229" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="230" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="231" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="232" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="233" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="234" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="235" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="236" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="237" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="238" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="239" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="240" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="241" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="242" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="243" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="244" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="245" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="246" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="247" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="248" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="249" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="250" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="251" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="252" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="253" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="254" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="255" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="256" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="257" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="258" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="259" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="260" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="261" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="262" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="263" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="264" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="265" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="266" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="267" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="268" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="269" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="270" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="271" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="272" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="273" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="274" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="275" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="276" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="277" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="278" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="279" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="280" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="281" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="282" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="283" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="285" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="286" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="287" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="288" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="289" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="290" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="291" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="292" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="34" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="293" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="294" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="295" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="34" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="296" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="34" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="297" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="298" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="299" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="34" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="300" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" s="34" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="301" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" s="34" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="302" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" s="34" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="303" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" s="34" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="304" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" s="34" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="305" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" s="34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="306" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" s="34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="307" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" s="34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="308" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" s="34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="309" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="310" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" s="34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="311" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="312" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" s="34" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="313" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="314" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" s="34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="315" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" s="34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="316" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" s="34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="317" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" s="34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="318" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" s="34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="319" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" s="34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="320" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" s="34" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="321" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" s="34" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="322" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" s="34" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="323" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" s="34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="324" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" s="34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="325" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" s="34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="326" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" s="34" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="327" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" s="34" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="328" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" s="34" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="329" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" s="34" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="330" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" s="34" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="331" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" s="34" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="332" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" s="34" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="333" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" s="34" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="334" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" s="34" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="335" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" s="34" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="336" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" s="34" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="337" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="34" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="338" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" s="34" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="339" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" s="34" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="340" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="34" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="341" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" s="34" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="342" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" s="34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="343" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" s="34" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="344" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="345" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" s="34" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="346" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" s="34" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="347" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" s="34" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="348" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" s="34" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="349" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" s="34" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="350" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" s="34" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="351" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" s="34" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="352" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" s="34" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="353" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" s="34" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="354" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" s="34" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="355" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" s="34" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="356" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" s="34" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="357" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" s="34" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="358" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" s="34" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="359" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" s="34" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="360" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" s="34" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="361" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" s="34" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="362" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" s="34" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="363" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="34" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="364" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" s="34" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="365" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" s="34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="366" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="367" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="368" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" s="34" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="369" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A369" s="34" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="370" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A370" s="34" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="371" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A371" s="34" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="372" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A372" s="34" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="373" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A373" s="34" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="374" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A374" s="34" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="375" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A375" s="34" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="376" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A376" s="34" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="377" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A377" s="34" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="378" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A378" s="34" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="379" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A379" s="34" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="380" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A380" s="34" t="s">
         <v>296</v>
       </c>
@@ -6436,20 +6276,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="P1:P380">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="SI"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -6464,6 +6291,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W43:W46">

</xml_diff>

<commit_message>
Asignación de autores escaleta mat 7 tema 11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion11/ESCALETA MA_07_11_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion11/ESCALETA MA_07_11_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvelasquez\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="390">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1188,6 +1188,12 @@
   </si>
   <si>
     <t>Aplica el Teorema de Pitágoras</t>
+  </si>
+  <si>
+    <t>Andrés Gómez</t>
+  </si>
+  <si>
+    <t>Joan Florez</t>
   </si>
 </sst>
 </file>
@@ -1676,22 +1682,13 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1737,6 +1734,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2046,8 +2052,8 @@
   <dimension ref="A1:X381"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2073,100 +2079,100 @@
     <col min="19" max="19" width="20.7109375" style="72" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="25.85546875" style="72" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="21.7109375" style="72" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="4"/>
+    <col min="22" max="22" width="16" style="4" customWidth="1"/>
     <col min="23" max="24" width="11.42578125" style="5"/>
     <col min="25" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="93" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="83" t="s">
+      <c r="H1" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="I1" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="93" t="s">
+      <c r="J1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="91" t="s">
+      <c r="K1" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="95" t="s">
+      <c r="M1" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="95"/>
-      <c r="O1" s="79" t="s">
+      <c r="N1" s="92"/>
+      <c r="O1" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="P1" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="80" t="s">
+      <c r="Q1" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="82" t="s">
+      <c r="R1" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="80" t="s">
+      <c r="S1" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="81" t="s">
+      <c r="T1" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="80" t="s">
+      <c r="U1" s="97" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="90"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="87"/>
       <c r="M2" s="3" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="80"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="97"/>
     </row>
     <row r="3" spans="1:24" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -2877,8 +2883,8 @@
       <c r="U13" s="64" t="s">
         <v>302</v>
       </c>
-      <c r="V13" s="4" t="s">
-        <v>373</v>
+      <c r="V13" s="49" t="s">
+        <v>388</v>
       </c>
       <c r="W13" s="16"/>
       <c r="X13" s="16"/>
@@ -3010,7 +3016,7 @@
         <v>294</v>
       </c>
       <c r="V15" s="49" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
@@ -3140,7 +3146,7 @@
         <v>294</v>
       </c>
       <c r="V17" s="49" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="W17" s="16"/>
       <c r="X17" s="16"/>
@@ -4903,7 +4909,7 @@
         <v>300</v>
       </c>
       <c r="V46" s="49" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="W46" s="16"/>
       <c r="X46" s="16"/>
@@ -6293,6 +6299,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -6307,12 +6319,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W43:W46">

</xml_diff>